<commit_message>
consolidate user access control
</commit_message>
<xml_diff>
--- a/protected/data/master/user.xlsx
+++ b/protected/data/master/user.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="228" yWindow="552" windowWidth="18876" windowHeight="8676"/>
+    <workbookView xWindow="228" yWindow="552" windowWidth="18876" windowHeight="8676" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="master" sheetId="1" r:id="rId1"/>
@@ -94,6 +94,29 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is referenced in the user profile lookup on the master worksheet</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="317">
   <si>
@@ -856,9 +879,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Create User, Edit Perm Group</t>
-  </si>
-  <si>
     <t>ECO Admin and Item Status</t>
   </si>
   <si>
@@ -871,34 +891,7 @@
     <t>Item User 6-10</t>
   </si>
   <si>
-    <t>Costs +  Update Costs when making Purch List</t>
-  </si>
-  <si>
-    <t>Sources (vendor, mfr, mfr pn, line card)</t>
-  </si>
-  <si>
-    <t>Cust &amp; Jobs (View)</t>
-  </si>
-  <si>
-    <t>Cust (Edit)</t>
-  </si>
-  <si>
-    <t>Job</t>
-  </si>
-  <si>
-    <t>PO</t>
-  </si>
-  <si>
-    <t>RFQ</t>
-  </si>
-  <si>
     <t>Overkit Entries</t>
-  </si>
-  <si>
-    <t>Min Stk Entries</t>
-  </si>
-  <si>
-    <t>Stock Qtys</t>
   </si>
   <si>
     <t>Units of Measure</t>
@@ -1056,6 +1049,36 @@
   </si>
   <si>
     <t>Export in CSV format to user.csv (note passwords are in plain text, use appropriate security measures)</t>
+  </si>
+  <si>
+    <t>Costs +  Update Costs when making Purch Lists</t>
+  </si>
+  <si>
+    <t>Sources: Vendors, Mfrs, Mfr P/Ns, Linecard</t>
+  </si>
+  <si>
+    <t>Customers/Jobs (View)</t>
+  </si>
+  <si>
+    <t>Customsers (Edit)</t>
+  </si>
+  <si>
+    <t>Jobs</t>
+  </si>
+  <si>
+    <t>Purchase Orders</t>
+  </si>
+  <si>
+    <t>Requests for Quotation</t>
+  </si>
+  <si>
+    <t>Minimum Stock Entries</t>
+  </si>
+  <si>
+    <t>Stock Quantities</t>
+  </si>
+  <si>
+    <t>Permission Groups, Group Members, ECO Departents, Users/Passwords.</t>
   </si>
 </sst>
 </file>
@@ -1401,15 +1424,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1446,6 +1460,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -1760,7 +1783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1871,7 +1894,7 @@
       <c r="AB6" s="15"/>
       <c r="AC6" s="16"/>
       <c r="AD6" s="16"/>
-      <c r="AE6" s="39"/>
+      <c r="AE6" s="36"/>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7" s="19"/>
@@ -1883,10 +1906,10 @@
         <v>10</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>11</v>
@@ -1960,7 +1983,7 @@
       <c r="AD7" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="AE7" s="40" t="s">
+      <c r="AE7" s="37" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1979,7 +2002,7 @@
       </c>
       <c r="E8" s="16"/>
       <c r="F8" s="16" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="17" t="s">
@@ -2000,10 +2023,10 @@
         <v>49</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="O8" s="7" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="P8" s="15"/>
       <c r="Q8" s="15"/>
@@ -2020,7 +2043,7 @@
       <c r="AB8" s="15"/>
       <c r="AC8" s="16"/>
       <c r="AD8" s="16"/>
-      <c r="AE8" s="39"/>
+      <c r="AE8" s="36"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9" s="23">
@@ -2058,10 +2081,10 @@
         <v>49</v>
       </c>
       <c r="N9" s="9" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="P9" s="9"/>
       <c r="Q9" s="9"/>
@@ -2078,7 +2101,7 @@
       <c r="AB9" s="9"/>
       <c r="AC9" s="25"/>
       <c r="AD9" s="25"/>
-      <c r="AE9" s="41"/>
+      <c r="AE9" s="38"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
@@ -2097,7 +2120,7 @@
       <c r="F10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="43">
         <v>21551</v>
       </c>
       <c r="H10" s="8" t="s">
@@ -2171,7 +2194,7 @@
       <c r="AD10" s="5">
         <v>13054</v>
       </c>
-      <c r="AE10" s="41" t="s">
+      <c r="AE10" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2192,7 +2215,7 @@
       <c r="F11" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="G11" s="46">
+      <c r="G11" s="43">
         <v>14277</v>
       </c>
       <c r="H11" s="8" t="s">
@@ -2263,7 +2286,7 @@
       <c r="AD11" s="5">
         <v>13054</v>
       </c>
-      <c r="AE11" s="41" t="s">
+      <c r="AE11" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2284,7 +2307,7 @@
       <c r="F12" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G12" s="46">
+      <c r="G12" s="43">
         <v>21610</v>
       </c>
       <c r="H12" s="8" t="s">
@@ -2358,7 +2381,7 @@
       <c r="AD12" s="5">
         <v>13054</v>
       </c>
-      <c r="AE12" s="41" t="s">
+      <c r="AE12" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2379,7 +2402,7 @@
       <c r="F13" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="G13" s="46">
+      <c r="G13" s="43">
         <v>21641</v>
       </c>
       <c r="H13" s="8" t="s">
@@ -2453,7 +2476,7 @@
       <c r="AD13" s="5">
         <v>13054</v>
       </c>
-      <c r="AE13" s="41" t="s">
+      <c r="AE13" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2474,7 +2497,7 @@
       <c r="F14" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="G14" s="46">
+      <c r="G14" s="43">
         <v>21671</v>
       </c>
       <c r="H14" s="8" t="s">
@@ -2548,7 +2571,7 @@
       <c r="AD14" s="5">
         <v>13054</v>
       </c>
-      <c r="AE14" s="41" t="s">
+      <c r="AE14" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2569,7 +2592,7 @@
       <c r="F15" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="G15" s="46">
+      <c r="G15" s="43">
         <v>21702</v>
       </c>
       <c r="H15" s="8" t="s">
@@ -2643,7 +2666,7 @@
       <c r="AD15" s="5">
         <v>13054</v>
       </c>
-      <c r="AE15" s="41" t="s">
+      <c r="AE15" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2664,7 +2687,7 @@
       <c r="F16" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="G16" s="46">
+      <c r="G16" s="43">
         <v>21732</v>
       </c>
       <c r="H16" s="8" t="s">
@@ -2738,7 +2761,7 @@
       <c r="AD16" s="5">
         <v>13054</v>
       </c>
-      <c r="AE16" s="41" t="s">
+      <c r="AE16" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2759,7 +2782,7 @@
       <c r="F17" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="G17" s="46">
+      <c r="G17" s="43">
         <v>21763</v>
       </c>
       <c r="H17" s="8" t="s">
@@ -2833,7 +2856,7 @@
       <c r="AD17" s="5">
         <v>13054</v>
       </c>
-      <c r="AE17" s="41" t="s">
+      <c r="AE17" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2854,7 +2877,7 @@
       <c r="F18" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="G18" s="46">
+      <c r="G18" s="43">
         <v>21794</v>
       </c>
       <c r="H18" s="8" t="s">
@@ -2928,7 +2951,7 @@
       <c r="AD18" s="5">
         <v>13054</v>
       </c>
-      <c r="AE18" s="41" t="s">
+      <c r="AE18" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2949,7 +2972,7 @@
       <c r="F19" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="46">
+      <c r="G19" s="43">
         <v>21824</v>
       </c>
       <c r="H19" s="8" t="s">
@@ -3023,7 +3046,7 @@
       <c r="AD19" s="5">
         <v>13054</v>
       </c>
-      <c r="AE19" s="41" t="s">
+      <c r="AE19" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3044,7 +3067,7 @@
       <c r="F20" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="G20" s="46">
+      <c r="G20" s="43">
         <v>21855</v>
       </c>
       <c r="H20" s="8" t="s">
@@ -3118,7 +3141,7 @@
       <c r="AD20" s="5">
         <v>13054</v>
       </c>
-      <c r="AE20" s="41" t="s">
+      <c r="AE20" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3139,7 +3162,7 @@
       <c r="F21" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="G21" s="46">
+      <c r="G21" s="43">
         <v>21885</v>
       </c>
       <c r="H21" s="8" t="s">
@@ -3213,7 +3236,7 @@
       <c r="AD21" s="5">
         <v>13054</v>
       </c>
-      <c r="AE21" s="41" t="s">
+      <c r="AE21" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3234,7 +3257,7 @@
       <c r="F22" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G22" s="46">
+      <c r="G22" s="43">
         <v>12785</v>
       </c>
       <c r="H22" s="8" t="s">
@@ -3308,7 +3331,7 @@
       <c r="AD22" s="5">
         <v>13054</v>
       </c>
-      <c r="AE22" s="41" t="s">
+      <c r="AE22" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3329,7 +3352,7 @@
       <c r="F23" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G23" s="46">
+      <c r="G23" s="43">
         <v>23815</v>
       </c>
       <c r="H23" s="8" t="s">
@@ -3403,7 +3426,7 @@
       <c r="AD23" s="5">
         <v>13054</v>
       </c>
-      <c r="AE23" s="41" t="s">
+      <c r="AE23" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3424,7 +3447,7 @@
       <c r="F24" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G24" s="46">
+      <c r="G24" s="43">
         <v>21976</v>
       </c>
       <c r="H24" s="8" t="s">
@@ -3498,7 +3521,7 @@
       <c r="AD24" s="5">
         <v>13054</v>
       </c>
-      <c r="AE24" s="41" t="s">
+      <c r="AE24" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3519,7 +3542,7 @@
       <c r="F25" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G25" s="46">
+      <c r="G25" s="43">
         <v>22007</v>
       </c>
       <c r="H25" s="8" t="s">
@@ -3593,7 +3616,7 @@
       <c r="AD25" s="5">
         <v>13054</v>
       </c>
-      <c r="AE25" s="41" t="s">
+      <c r="AE25" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3614,7 +3637,7 @@
       <c r="F26" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="G26" s="46">
+      <c r="G26" s="43">
         <v>22037</v>
       </c>
       <c r="H26" s="8" t="s">
@@ -3688,7 +3711,7 @@
       <c r="AD26" s="5">
         <v>13054</v>
       </c>
-      <c r="AE26" s="41" t="s">
+      <c r="AE26" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3709,7 +3732,7 @@
       <c r="F27" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="G27" s="46">
+      <c r="G27" s="43">
         <v>13667</v>
       </c>
       <c r="H27" s="8" t="s">
@@ -3783,7 +3806,7 @@
       <c r="AD27" s="5">
         <v>13054</v>
       </c>
-      <c r="AE27" s="41" t="s">
+      <c r="AE27" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3804,7 +3827,7 @@
       <c r="F28" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="G28" s="46">
+      <c r="G28" s="43">
         <v>22098</v>
       </c>
       <c r="H28" s="8" t="s">
@@ -3878,7 +3901,7 @@
       <c r="AD28" s="5">
         <v>13054</v>
       </c>
-      <c r="AE28" s="41" t="s">
+      <c r="AE28" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3899,7 +3922,7 @@
       <c r="F29" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="G29" s="46">
+      <c r="G29" s="43">
         <v>21879</v>
       </c>
       <c r="H29" s="8" t="s">
@@ -3973,7 +3996,7 @@
       <c r="AD29" s="5">
         <v>13054</v>
       </c>
-      <c r="AE29" s="41" t="s">
+      <c r="AE29" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3994,7 +4017,7 @@
       <c r="F30" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="G30" s="46">
+      <c r="G30" s="43">
         <v>22160</v>
       </c>
       <c r="H30" s="8" t="s">
@@ -4068,7 +4091,7 @@
       <c r="AD30" s="5">
         <v>13054</v>
       </c>
-      <c r="AE30" s="41" t="s">
+      <c r="AE30" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4089,7 +4112,7 @@
       <c r="F31" s="25" t="s">
         <v>226</v>
       </c>
-      <c r="G31" s="46">
+      <c r="G31" s="43">
         <v>22190</v>
       </c>
       <c r="H31" s="8" t="s">
@@ -4163,7 +4186,7 @@
       <c r="AD31" s="25">
         <v>13054</v>
       </c>
-      <c r="AE31" s="41" t="s">
+      <c r="AE31" s="38" t="s">
         <v>58</v>
       </c>
     </row>
@@ -5290,7 +5313,7 @@
       <c r="J2" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="47" t="str">
+      <c r="K2" s="44" t="str">
         <f>CONCATENATE(A2,":",B2,":",C2,":",D2,":",E2,":",F2,":",G2,":",H2,":",I2,":",J2)</f>
         <v>admin::::::Admin User, Maestro Administrator::tcsh:admin</v>
       </c>
@@ -5309,7 +5332,7 @@
       <c r="J3" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="47" t="str">
+      <c r="K3" s="44" t="str">
         <f t="shared" ref="K3:K25" si="0">CONCATENATE(A3,":",B3,":",C3,":",D3,":",E3,":",F3,":",G3,":",H3,":",I3,":",J3)</f>
         <v>demo::::::Demo User, Maestro Demonstrator::tcsh:demo</v>
       </c>
@@ -5328,7 +5351,7 @@
       <c r="J4" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="47" t="str">
+      <c r="K4" s="44" t="str">
         <f t="shared" si="0"/>
         <v>bjenks::::::Barcoe Jenks, Electronics Engineer::tcsh:appleton</v>
       </c>
@@ -5347,7 +5370,7 @@
       <c r="J5" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K5" s="47" t="str">
+      <c r="K5" s="44" t="str">
         <f t="shared" si="0"/>
         <v>bswift::::::Barton Swift, President::tcsh:appleton</v>
       </c>
@@ -5366,7 +5389,7 @@
       <c r="J6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="47" t="str">
+      <c r="K6" s="44" t="str">
         <f t="shared" si="0"/>
         <v>barmstrong::::::Bub Armstrong, Mechanical Engineer::tcsh:appleton</v>
       </c>
@@ -5385,7 +5408,7 @@
       <c r="J7" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="47" t="str">
+      <c r="K7" s="44" t="str">
         <f t="shared" si="0"/>
         <v>fmason::::::Frank Mason, Engineering Project Coordinator::tcsh:appleton</v>
       </c>
@@ -5404,7 +5427,7 @@
       <c r="J8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="47" t="str">
+      <c r="K8" s="44" t="str">
         <f t="shared" si="0"/>
         <v>gjackson::::::Garret Jackson, Production Planner::tcsh:appleton</v>
       </c>
@@ -5423,7 +5446,7 @@
       <c r="J9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="47" t="str">
+      <c r="K9" s="44" t="str">
         <f t="shared" si="0"/>
         <v>hbaldwin::::::Hank Baldwin, Lead Hand::tcsh:appleton</v>
       </c>
@@ -5442,7 +5465,7 @@
       <c r="J10" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K10" s="47" t="str">
+      <c r="K10" s="44" t="str">
         <f t="shared" si="0"/>
         <v>hrandall::::::Helen Randall, AP Clerk::tcsh:appleton</v>
       </c>
@@ -5461,7 +5484,7 @@
       <c r="J11" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K11" s="47" t="str">
+      <c r="K11" s="44" t="str">
         <f t="shared" si="0"/>
         <v>jwood::::::Jacab Wood, Sales Agent::tcsh:appleton</v>
       </c>
@@ -5480,7 +5503,7 @@
       <c r="J12" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K12" s="47" t="str">
+      <c r="K12" s="44" t="str">
         <f t="shared" si="0"/>
         <v>jperiod::::::James Period, Director, Sales &amp; Marketing::tcsh:appleton</v>
       </c>
@@ -5499,7 +5522,7 @@
       <c r="J13" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K13" s="47" t="str">
+      <c r="K13" s="44" t="str">
         <f t="shared" si="0"/>
         <v>jhaddon::::::Jennie Haddon, Buyer::tcsh:appleton</v>
       </c>
@@ -5518,7 +5541,7 @@
       <c r="J14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="47" t="str">
+      <c r="K14" s="44" t="str">
         <f t="shared" si="0"/>
         <v>jmorse::::::Jennie Morse, AR Clerk::tcsh:appleton</v>
       </c>
@@ -5537,7 +5560,7 @@
       <c r="J15" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K15" s="47" t="str">
+      <c r="K15" s="44" t="str">
         <f t="shared" si="0"/>
         <v>jsharp::::::John Sharp, Director, Prod Mgmt::tcsh:appleton</v>
       </c>
@@ -5556,7 +5579,7 @@
       <c r="J16" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K16" s="47" t="str">
+      <c r="K16" s="44" t="str">
         <f t="shared" si="0"/>
         <v>mbaggert::::::Martha Baggert, Director, Human Resources::tcsh:appleton</v>
       </c>
@@ -5575,7 +5598,7 @@
       <c r="J17" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K17" s="47" t="str">
+      <c r="K17" s="44" t="str">
         <f t="shared" si="0"/>
         <v>mnestor::::::Mary Nestor, Director, MIS-IT::tcsh:appleton</v>
       </c>
@@ -5594,7 +5617,7 @@
       <c r="J18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K18" s="47" t="str">
+      <c r="K18" s="44" t="str">
         <f t="shared" si="0"/>
         <v>mblair::::::Minnie Blair, Software Engineer::tcsh:appleton</v>
       </c>
@@ -5613,7 +5636,7 @@
       <c r="J19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K19" s="47" t="str">
+      <c r="K19" s="44" t="str">
         <f t="shared" si="0"/>
         <v>mdelazes::::::Miquel DeLazes, Director, Manufacturing::tcsh:appleton</v>
       </c>
@@ -5632,7 +5655,7 @@
       <c r="J20" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K20" s="47" t="str">
+      <c r="K20" s="44" t="str">
         <f t="shared" si="0"/>
         <v>nnewton::::::Ned Newton, Chief Financial Officer::tcsh:appleton</v>
       </c>
@@ -5651,7 +5674,7 @@
       <c r="J21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K21" s="47" t="str">
+      <c r="K21" s="44" t="str">
         <f t="shared" si="0"/>
         <v>rsampson::::::Rad Sampson, Director, Quality::tcsh:appleton</v>
       </c>
@@ -5670,7 +5693,7 @@
       <c r="J22" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K22" s="47" t="str">
+      <c r="K22" s="44" t="str">
         <f t="shared" si="0"/>
         <v>smalloy::::::Sarah Malloy, Receiver::tcsh:appleton</v>
       </c>
@@ -5689,7 +5712,7 @@
       <c r="J23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K23" s="47" t="str">
+      <c r="K23" s="44" t="str">
         <f t="shared" si="0"/>
         <v>tswift::::::Tom Swift, Director, Engineering::tcsh:appleton</v>
       </c>
@@ -5708,7 +5731,7 @@
       <c r="J24" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K24" s="47" t="str">
+      <c r="K24" s="44" t="str">
         <f t="shared" si="0"/>
         <v>wdamon::::::Wakefield Damon, Technical Writer::tcsh:appleton</v>
       </c>
@@ -5727,7 +5750,7 @@
       <c r="J25" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="K25" s="47" t="str">
+      <c r="K25" s="44" t="str">
         <f t="shared" si="0"/>
         <v>wcrawford::::::William Crawford, Director, Legal::tcsh:appleton</v>
       </c>
@@ -5761,34 +5784,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="J1" s="44" t="s">
-        <v>292</v>
+      <c r="J1" s="41" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -5813,17 +5836,17 @@
         <v>admin@swiftconstructioncompany.net</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I2" s="7" t="str">
         <f>master!H8</f>
         <v>admin</v>
       </c>
-      <c r="J2" s="45" t="s">
-        <v>296</v>
+      <c r="J2" s="42" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -5848,17 +5871,17 @@
         <v>admin@swiftconstructioncompany.net</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I3" s="7" t="str">
         <f>master!H9</f>
         <v>demo</v>
       </c>
-      <c r="J3" s="42" t="s">
-        <v>297</v>
+      <c r="J3" s="39" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -5887,16 +5910,16 @@
         <v>cn=Tom Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I4" s="7" t="str">
         <f>master!H10</f>
         <v>bjenks</v>
       </c>
-      <c r="J4" s="43" t="s">
+      <c r="J4" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5922,16 +5945,16 @@
         <v>bswift@swiftconstructioncompany.net</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I5" s="7" t="str">
         <f>master!H11</f>
         <v>bswift</v>
       </c>
-      <c r="J5" s="43" t="s">
+      <c r="J5" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5961,16 +5984,16 @@
         <v>cn=Tom Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I6" s="7" t="str">
         <f>master!H12</f>
         <v>barmstrong</v>
       </c>
-      <c r="J6" s="43" t="s">
+      <c r="J6" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6000,16 +6023,16 @@
         <v>cn=Tom Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I7" s="7" t="str">
         <f>master!H13</f>
         <v>fmason</v>
       </c>
-      <c r="J7" s="43" t="s">
+      <c r="J7" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6039,16 +6062,16 @@
         <v>cn=Miguel DeLazes,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I8" s="7" t="str">
         <f>master!H14</f>
         <v>gjackson</v>
       </c>
-      <c r="J8" s="43" t="s">
+      <c r="J8" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6078,16 +6101,16 @@
         <v>cn=Miguel DeLazes,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I9" s="7" t="str">
         <f>master!H15</f>
         <v>hbaldwin</v>
       </c>
-      <c r="J9" s="43" t="s">
+      <c r="J9" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6117,16 +6140,16 @@
         <v>cn=Ned Newton,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I10" s="7" t="str">
         <f>master!H16</f>
         <v>hrandall</v>
       </c>
-      <c r="J10" s="43" t="s">
+      <c r="J10" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6156,16 +6179,16 @@
         <v>cn=James Period,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I11" s="7" t="str">
         <f>master!H17</f>
         <v>jwood</v>
       </c>
-      <c r="J11" s="43" t="s">
+      <c r="J11" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6195,16 +6218,16 @@
         <v>cn=Barton Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I12" s="7" t="str">
         <f>master!H18</f>
         <v>jperiod</v>
       </c>
-      <c r="J12" s="43" t="s">
+      <c r="J12" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6234,16 +6257,16 @@
         <v>cn=Miguel DeLazes,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I13" s="7" t="str">
         <f>master!H19</f>
         <v>jhaddon</v>
       </c>
-      <c r="J13" s="43" t="s">
+      <c r="J13" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6273,16 +6296,16 @@
         <v>cn=Ned Newton,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I14" s="7" t="str">
         <f>master!H20</f>
         <v>jmorse</v>
       </c>
-      <c r="J14" s="43" t="s">
+      <c r="J14" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6312,16 +6335,16 @@
         <v>cn=Barton Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I15" s="7" t="str">
         <f>master!H21</f>
         <v>jsharp</v>
       </c>
-      <c r="J15" s="43" t="s">
+      <c r="J15" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6351,16 +6374,16 @@
         <v>cn=Barton Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I16" s="7" t="str">
         <f>master!H22</f>
         <v>mbaggert</v>
       </c>
-      <c r="J16" s="43" t="s">
+      <c r="J16" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6390,16 +6413,16 @@
         <v>cn=Barton Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I17" s="7" t="str">
         <f>master!H23</f>
         <v>mnestor</v>
       </c>
-      <c r="J17" s="43" t="s">
+      <c r="J17" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6429,16 +6452,16 @@
         <v>cn=Tom Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I18" s="7" t="str">
         <f>master!H24</f>
         <v>mblair</v>
       </c>
-      <c r="J18" s="43" t="s">
+      <c r="J18" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6468,16 +6491,16 @@
         <v>cn=Barton Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I19" s="7" t="str">
         <f>master!H25</f>
         <v>mdelazes</v>
       </c>
-      <c r="J19" s="43" t="s">
+      <c r="J19" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6507,16 +6530,16 @@
         <v>cn=Barton Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H20" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I20" s="7" t="str">
         <f>master!H26</f>
         <v>nnewton</v>
       </c>
-      <c r="J20" s="43" t="s">
+      <c r="J20" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6546,16 +6569,16 @@
         <v>cn=Barton Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I21" s="7" t="str">
         <f>master!H27</f>
         <v>rsampson</v>
       </c>
-      <c r="J21" s="43" t="s">
+      <c r="J21" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6585,16 +6608,16 @@
         <v>cn=Miguel DeLazes,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I22" s="7" t="str">
         <f>master!H28</f>
         <v>smalloy</v>
       </c>
-      <c r="J22" s="43" t="s">
+      <c r="J22" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6624,16 +6647,16 @@
         <v>cn=Barton Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I23" s="7" t="str">
         <f>master!H29</f>
         <v>tswift</v>
       </c>
-      <c r="J23" s="43" t="s">
+      <c r="J23" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6663,16 +6686,16 @@
         <v>cn=John Sharp,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G24" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I24" s="7" t="str">
         <f>master!H30</f>
         <v>wdamon</v>
       </c>
-      <c r="J24" s="43" t="s">
+      <c r="J24" s="40" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6702,16 +6725,16 @@
         <v>cn=Barton Swift,ou=People,dc=root,dc=org</v>
       </c>
       <c r="G25" s="7" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="I25" s="7" t="str">
         <f>master!H31</f>
         <v>wcrawford</v>
       </c>
-      <c r="J25" s="42" t="s">
+      <c r="J25" s="39" t="s">
         <v>47</v>
       </c>
     </row>
@@ -6723,21 +6746,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="34" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="31" customWidth="1"/>
     <col min="2" max="2" width="13.19921875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="41.69921875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="6.69921875" style="35" customWidth="1"/>
-    <col min="5" max="24" width="6.69921875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="46.296875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="6.69921875" style="32" customWidth="1"/>
+    <col min="5" max="24" width="5.69921875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="92.4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="171" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>3</v>
       </c>
@@ -6750,152 +6776,152 @@
       <c r="D1" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="45" t="s">
+        <v>316</v>
+      </c>
+      <c r="F1" s="46" t="s">
         <v>253</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="G1" s="46" t="s">
         <v>254</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="H1" s="46" t="s">
         <v>255</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="I1" s="46" t="s">
         <v>256</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="J1" s="46" t="s">
+        <v>307</v>
+      </c>
+      <c r="K1" s="46" t="s">
+        <v>308</v>
+      </c>
+      <c r="L1" s="46" t="s">
+        <v>309</v>
+      </c>
+      <c r="M1" s="46" t="s">
+        <v>310</v>
+      </c>
+      <c r="N1" s="46" t="s">
+        <v>311</v>
+      </c>
+      <c r="O1" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="P1" s="46" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q1" s="46" t="s">
         <v>257</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="R1" s="46" t="s">
+        <v>314</v>
+      </c>
+      <c r="S1" s="46" t="s">
+        <v>315</v>
+      </c>
+      <c r="T1" s="46" t="s">
         <v>258</v>
       </c>
-      <c r="K1" s="30" t="s">
+      <c r="U1" s="46" t="s">
         <v>259</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="V1" s="46" t="s">
         <v>260</v>
       </c>
-      <c r="M1" s="30" t="s">
+      <c r="W1" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="X1" s="47" t="s">
         <v>262</v>
       </c>
-      <c r="O1" s="30" t="s">
-        <v>263</v>
-      </c>
-      <c r="P1" s="30" t="s">
-        <v>264</v>
-      </c>
-      <c r="Q1" s="30" t="s">
-        <v>265</v>
-      </c>
-      <c r="R1" s="30" t="s">
-        <v>266</v>
-      </c>
-      <c r="S1" s="30" t="s">
-        <v>267</v>
-      </c>
-      <c r="T1" s="30" t="s">
-        <v>268</v>
-      </c>
-      <c r="U1" s="30" t="s">
-        <v>269</v>
-      </c>
-      <c r="V1" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="W1" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="X1" s="31" t="s">
-        <v>272</v>
-      </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="32">
+      <c r="A2" s="29">
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="D2" s="33">
+      <c r="C2" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="D2" s="30">
         <v>1</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="P2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="W2" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="X2" s="33" t="s">
-        <v>274</v>
+        <v>264</v>
+      </c>
+      <c r="X2" s="30" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="32">
+      <c r="A3" s="29">
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="D3" s="33">
+      <c r="C3" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" s="30">
         <v>2</v>
       </c>
       <c r="E3" s="6"/>
@@ -6906,7 +6932,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
@@ -6917,85 +6943,85 @@
       <c r="S3" s="6"/>
       <c r="T3" s="6"/>
       <c r="U3" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="V3" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="W3" s="6"/>
-      <c r="X3" s="33" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" s="32">
+      <c r="X3" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="29">
         <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="D4" s="33">
+      <c r="C4" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="D4" s="30">
         <v>3</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="U4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="V4" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="X4" s="33" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A5" s="32">
+        <v>264</v>
+      </c>
+      <c r="X4" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="29">
         <v>4</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="D5" s="33">
+      <c r="C5" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="D5" s="30">
         <v>4</v>
       </c>
       <c r="E5" s="6"/>
@@ -7005,19 +7031,19 @@
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -7025,27 +7051,27 @@
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="V5" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="W5" s="6"/>
-      <c r="X5" s="33" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+      <c r="X5" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
         <v>5</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="D6" s="33">
+      <c r="C6" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="D6" s="30">
         <v>5</v>
       </c>
       <c r="E6" s="6"/>
@@ -7056,43 +7082,43 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="T6" s="6"/>
       <c r="U6" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="V6" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="X6" s="33" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="32">
+        <v>264</v>
+      </c>
+      <c r="X6" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A7" s="29">
         <v>6</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="D7" s="33">
+      <c r="C7" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="D7" s="30">
         <v>6</v>
       </c>
       <c r="E7" s="6"/>
@@ -7100,58 +7126,58 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="K7" s="6"/>
       <c r="L7" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="Q7" s="6"/>
       <c r="R7" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="T7" s="6"/>
       <c r="U7" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="V7" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="W7" s="6"/>
-      <c r="X7" s="33" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" s="32">
+      <c r="X7" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="A8" s="29">
         <v>7</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>182</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D8" s="33">
+      <c r="C8" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="D8" s="30">
         <v>7</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
@@ -7159,7 +7185,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
@@ -7170,27 +7196,27 @@
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="V8" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="W8" s="6"/>
-      <c r="X8" s="33" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
+      <c r="X8" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="29">
         <v>8</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="D9" s="33">
+      <c r="C9" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D9" s="30">
         <v>8</v>
       </c>
       <c r="E9" s="6"/>
@@ -7201,13 +7227,13 @@
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -7216,27 +7242,27 @@
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="V9" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="W9" s="6"/>
-      <c r="X9" s="33" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="32">
+      <c r="X9" s="30" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
         <v>9</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="D10" s="33">
+      <c r="C10" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="D10" s="30">
         <v>9</v>
       </c>
       <c r="E10" s="6"/>
@@ -7247,7 +7273,7 @@
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
@@ -7258,22 +7284,24 @@
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="V10" s="6" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="W10" s="6"/>
-      <c r="X10" s="33" t="s">
-        <v>274</v>
+      <c r="X10" s="30" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:B10">
     <sortCondition ref="B2:B10"/>
   </sortState>
-  <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
-  <pageSetup fitToWidth="0" fitToHeight="0" pageOrder="overThenDown" orientation="portrait" r:id="rId1"/>
+  <printOptions gridLines="1"/>
+  <pageMargins left="0" right="0" top="0.39410000000000001" bottom="0.39410000000000001" header="0" footer="0"/>
+  <pageSetup paperSize="5" scale="86" pageOrder="overThenDown" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7295,10 +7323,10 @@
       <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="33" t="s">
         <v>251</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="33" t="s">
         <v>252</v>
       </c>
     </row>
@@ -7307,10 +7335,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>302</v>
+        <v>273</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -7318,10 +7346,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="C3" s="37" t="s">
-        <v>303</v>
+        <v>274</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -7342,23 +7370,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
-        <v>298</v>
+      <c r="A1" s="35" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
-        <v>314</v>
+      <c r="A5" s="35" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -7366,7 +7394,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -7374,12 +7402,12 @@
         <v>2</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
-        <v>304</v>
+      <c r="A9" s="35" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -7387,7 +7415,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -7395,7 +7423,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -7403,12 +7431,12 @@
         <v>3</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
-        <v>305</v>
+      <c r="A14" s="35" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -7416,7 +7444,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -7424,7 +7452,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -7432,7 +7460,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>

</xml_diff>